<commit_message>
sprint project update 2
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester7\code\project_pembelajaran_mesin_2018-198\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79BDE12-0149-42E9-AD01-2CE641375A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B3E335-453E-4F55-94CF-6326D4B12D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Data Preparation</t>
   </si>
@@ -37,44 +37,44 @@
     <t>bug fixing</t>
   </si>
   <si>
-    <t>activity</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>till semester exam</t>
-  </si>
-  <si>
-    <t>13/10/2021</t>
-  </si>
-  <si>
-    <t>19/10/2021</t>
-  </si>
-  <si>
-    <t>20/10/2021</t>
-  </si>
-  <si>
-    <t>28/10/2021</t>
-  </si>
-  <si>
-    <t>29/10/2021</t>
-  </si>
-  <si>
-    <t>15/11/2021</t>
-  </si>
-  <si>
-    <t>16/11/2021</t>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>13/10/2021 - 19/10/2021</t>
+  </si>
+  <si>
+    <t>20/10/2021-28/10/2021</t>
+  </si>
+  <si>
+    <t>29/10/2021-10/11/2021</t>
+  </si>
+  <si>
+    <t>11/11/2021-15/11/2021</t>
+  </si>
+  <si>
+    <t>16/11/2021-till semester exam</t>
+  </si>
+  <si>
+    <t>Time Line</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Not Yet</t>
+  </si>
+  <si>
+    <t>Penanggung Jawab</t>
+  </si>
+  <si>
+    <t>Ahmad Hanif Nurfauzi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -86,16 +86,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,19 +126,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -336,85 +391,138 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2">
-        <v>44480</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>44511</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>